<commit_message>
modificaciones en grandes cliente, y lecturas
</commit_message>
<xml_diff>
--- a/Lecturas_BureauVeritas/Lecturas_BureauVeritas/Upload/7_IMPORT_GRANDESCLIENTES_1.xlsx
+++ b/Lecturas_BureauVeritas/Lecturas_BureauVeritas/Upload/7_IMPORT_GRANDESCLIENTES_1.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Importar" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Importar!$A$1:$F$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Importar!$A$1:$F$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Codigo ERM</t>
   </si>
@@ -71,43 +71,13 @@
     <t>Instromet</t>
   </si>
   <si>
-    <t>Itron</t>
-  </si>
-  <si>
-    <t>EMR-16053</t>
-  </si>
-  <si>
-    <t>ES Caligas</t>
-  </si>
-  <si>
-    <t>PJ 31 308 Piso 1 Urb. ZONA INDUSTRIAL CERCADO DE LIMA LIMA</t>
-  </si>
-  <si>
-    <t>Gas Natural Vehicular</t>
-  </si>
-  <si>
-    <t>AV SANTIAGO DE SURCO 4080 Piso 1 Urb. 18 DE NOVIEMBRE SANTIAGO DE SURCO LIMA</t>
-  </si>
-  <si>
-    <t>SANTIAGO DE SURCO</t>
-  </si>
-  <si>
-    <t>EMR-16192</t>
-  </si>
-  <si>
-    <t>ES Marsano II</t>
-  </si>
-  <si>
-    <t>correo electronico</t>
-  </si>
-  <si>
-    <t>david.dsige@gmail.com</t>
-  </si>
-  <si>
-    <t>irvin.dsige@gmail.com</t>
-  </si>
-  <si>
-    <t>jhonny.apm12@gmail.com</t>
+    <t>correo copia</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>cesar.languasco@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -187,12 +157,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -508,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,10 +497,11 @@
     <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="68.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,11 +520,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>21</v>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -566,63 +546,16 @@
       <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="H2" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G4" r:id="rId2" display="mailto:jhonny.apm12@gmail.com"/>
-    <hyperlink ref="G3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>